<commit_message>
fix: KeyError in method conductor_components_instance
KeyError: 'stabilizer_material'

modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_1_input.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_1_input.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_1_ITER_like_LTS/conductor_1_input.xlsx
+++ b/TDD_examples/CASE_1_ITER_like_LTS/conductor_1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_1_ITER_like_LTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C7DEF4-F48E-4598-B2DA-5D4C22C1E5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A668DBE0-59E8-4F8E-BBD2-F5B1F0945198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="1110" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="143">
   <si>
     <t>COSTETA</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>SIDE2</t>
-  </si>
-  <si>
-    <t>ISTABILIZER</t>
   </si>
   <si>
     <t>Z_JACKET</t>
@@ -972,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -985,7 +982,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="12">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1030,10 +1027,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6">
         <v>5.0265000000000001E-5</v>
@@ -1044,16 +1041,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -1064,16 +1061,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -1084,22 +1081,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,10 +1107,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="7">
         <v>8.0000000000000002E-3</v>
@@ -1124,16 +1121,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -1147,13 +1144,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1164,16 +1161,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -1187,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5">
         <v>-99</v>
@@ -1207,13 +1204,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="5">
         <v>0.02</v>
@@ -1227,10 +1224,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="5" t="b">
         <f>FALSE</f>
@@ -1249,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="6">
         <v>0</v>
@@ -1266,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="6">
         <v>0</v>
@@ -1277,36 +1274,36 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1317,16 +1314,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E19" s="5" t="b">
         <v>0</v>
@@ -1365,7 +1362,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
@@ -1373,7 +1370,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="9">
         <v>0</v>
@@ -1384,7 +1381,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1421,10 +1418,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="11">
         <v>0</v>
@@ -1432,16 +1429,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -1449,16 +1446,16 @@
     </row>
     <row r="6" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -1469,13 +1466,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -1483,16 +1480,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
@@ -1500,196 +1497,196 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="6">
         <v>170360000000000</v>
@@ -1697,16 +1694,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="5">
         <v>30.23</v>
@@ -1714,16 +1711,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="E23" s="5">
         <v>16.73</v>
@@ -1731,16 +1728,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="E24" s="5">
         <v>20</v>
@@ -1748,16 +1745,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="E25" s="5">
         <f>10^-5</f>
@@ -1766,16 +1763,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="5" t="b">
         <v>1</v>
@@ -1819,7 +1816,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="9">
         <v>1</v>
@@ -1830,7 +1827,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1867,10 +1864,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" s="6">
         <f>(0.00052534+0.00025201)*E7</f>
@@ -1879,16 +1876,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -1896,16 +1893,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -1916,13 +1913,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -1930,16 +1927,16 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -1947,16 +1944,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="7">
         <v>2.0846</v>
@@ -1964,16 +1961,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="16">
         <v>2</v>
@@ -1981,16 +1978,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E11" s="5">
         <v>900</v>
@@ -1998,16 +1995,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="5">
         <f>0.000822</f>
@@ -2016,16 +2013,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="E13" s="5">
         <v>522</v>
@@ -2033,16 +2030,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" s="5">
         <f>0.000821</f>
@@ -2051,19 +2048,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2071,13 +2068,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="16">
         <v>197.71</v>
@@ -2085,33 +2082,33 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2119,16 +2116,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="6">
         <v>121508000000</v>
@@ -2136,16 +2133,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="6">
         <v>32.35</v>
@@ -2153,16 +2150,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E21" s="6">
         <v>16.22</v>
@@ -2170,16 +2167,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="E22" s="5">
         <v>5</v>
@@ -2187,16 +2184,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="E23" s="5">
         <f>10^-5</f>
@@ -2205,16 +2202,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" s="5" t="b">
         <v>0</v>
@@ -2231,11 +2228,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD13407-BFB1-4787-A354-6C7A2E5E5AE6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD6"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2247,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
@@ -2258,7 +2255,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2">
         <v>0</v>
@@ -2269,7 +2266,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="12">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2306,10 +2303,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="11">
         <v>0</v>
@@ -2317,16 +2314,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -2334,16 +2331,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -2354,13 +2351,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>0.96989999999999998</v>
@@ -2368,19 +2365,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,13 +2385,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="10">
         <v>100</v>
@@ -2402,16 +2399,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="5" t="b">
         <v>1</v>
@@ -2428,7 +2425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -2447,7 +2444,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="12">
         <f>SUM(E$2:Z2)</f>
@@ -2455,7 +2452,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="9">
         <v>1</v>
@@ -2466,7 +2463,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="13">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2497,16 +2494,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6">
         <f>0.00030699</f>
@@ -2515,16 +2512,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="6">
         <v>2.7965999999999999E-4</v>
@@ -2532,16 +2529,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -2549,16 +2546,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
@@ -2566,16 +2563,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="6">
         <v>0.1288</v>
@@ -2583,16 +2580,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="6">
         <v>0.13569999999999999</v>
@@ -2600,16 +2597,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
@@ -2617,36 +2614,36 @@
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,13 +2651,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
@@ -2668,33 +2665,33 @@
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="E14" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -2702,16 +2699,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>

</xml_diff>